<commit_message>
this update 2018-11-12,has deal with
</commit_message>
<xml_diff>
--- a/src/main/resources/templet/download/order/distributAskcost.xlsx
+++ b/src/main/resources/templet/download/order/distributAskcost.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>类别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,16 +48,13 @@
   <si>
     <t>图号</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>含税/未税</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +70,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="楷体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,27 +79,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -118,11 +93,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -426,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -438,11 +410,11 @@
     <col min="3" max="3" width="39.125" customWidth="1"/>
     <col min="4" max="4" width="32.75" customWidth="1"/>
     <col min="5" max="5" width="26.875" customWidth="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="11" max="11" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,10 +436,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>